<commit_message>
Adding a new column to the input file
</commit_message>
<xml_diff>
--- a/src/main/resources/Templates.xlsx
+++ b/src/main/resources/Templates.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MAP" sheetId="1" r:id="rId1"/>
@@ -141,22 +141,26 @@
     <font>
       <sz val="18"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -802,6 +806,45 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -816,45 +859,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1216,7 +1220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -1232,19 +1236,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="84"/>
-      <c r="E1" s="82" t="s">
+      <c r="B1" s="78"/>
+      <c r="C1" s="79"/>
+      <c r="E1" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="83"/>
-      <c r="G1" s="84"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="79"/>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="80"/>
+      <c r="A2" s="72"/>
       <c r="B2" s="74"/>
       <c r="C2" s="2" t="s">
         <v>1</v>
@@ -1258,7 +1262,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="85"/>
+      <c r="A3" s="80"/>
       <c r="B3" s="75"/>
       <c r="C3" s="3"/>
       <c r="E3" s="29"/>
@@ -1266,7 +1270,7 @@
       <c r="G3" s="30"/>
     </row>
     <row r="4" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="86"/>
+      <c r="A4" s="81"/>
       <c r="B4" s="75"/>
       <c r="C4" s="4">
         <v>52782</v>
@@ -1284,64 +1288,64 @@
         <v>2</v>
       </c>
       <c r="B5" s="75"/>
-      <c r="C5" s="69"/>
+      <c r="C5" s="82"/>
       <c r="E5" s="33" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="75"/>
-      <c r="G5" s="69"/>
+      <c r="G5" s="82"/>
     </row>
     <row r="6" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="75"/>
-      <c r="C6" s="70"/>
+      <c r="C6" s="83"/>
       <c r="E6" s="34"/>
       <c r="F6" s="75"/>
-      <c r="G6" s="70"/>
+      <c r="G6" s="83"/>
     </row>
     <row r="7" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>52812</v>
       </c>
       <c r="B7" s="75"/>
-      <c r="C7" s="70"/>
+      <c r="C7" s="83"/>
       <c r="E7" s="35">
         <v>52679</v>
       </c>
       <c r="F7" s="75"/>
-      <c r="G7" s="70"/>
+      <c r="G7" s="83"/>
     </row>
     <row r="8" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="75"/>
-      <c r="C8" s="70"/>
+      <c r="C8" s="83"/>
       <c r="E8" s="36" t="s">
         <v>3</v>
       </c>
       <c r="F8" s="75"/>
-      <c r="G8" s="70"/>
+      <c r="G8" s="83"/>
     </row>
     <row r="9" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="75"/>
-      <c r="C9" s="70"/>
+      <c r="C9" s="83"/>
       <c r="E9" s="37"/>
       <c r="F9" s="75"/>
-      <c r="G9" s="70"/>
+      <c r="G9" s="83"/>
     </row>
     <row r="10" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <v>52728</v>
       </c>
       <c r="B10" s="75"/>
-      <c r="C10" s="71"/>
+      <c r="C10" s="84"/>
       <c r="E10" s="38">
         <v>52778</v>
       </c>
       <c r="F10" s="75"/>
-      <c r="G10" s="71"/>
+      <c r="G10" s="84"/>
     </row>
     <row r="11" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
@@ -1393,7 +1397,7 @@
         <v>9</v>
       </c>
       <c r="F14" s="75"/>
-      <c r="G14" s="69"/>
+      <c r="G14" s="82"/>
     </row>
     <row r="15" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19"/>
@@ -1401,7 +1405,7 @@
       <c r="C15" s="20"/>
       <c r="E15" s="46"/>
       <c r="F15" s="75"/>
-      <c r="G15" s="70"/>
+      <c r="G15" s="83"/>
     </row>
     <row r="16" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="21">
@@ -1413,7 +1417,7 @@
         <v>52780</v>
       </c>
       <c r="F16" s="75"/>
-      <c r="G16" s="70"/>
+      <c r="G16" s="83"/>
     </row>
     <row r="17" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
@@ -1427,20 +1431,20 @@
         <v>4</v>
       </c>
       <c r="F17" s="75"/>
-      <c r="G17" s="70"/>
+      <c r="G17" s="83"/>
     </row>
     <row r="18" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="77" t="s">
+      <c r="A18" s="69" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="75"/>
       <c r="C18" s="24"/>
       <c r="E18" s="49"/>
       <c r="F18" s="75"/>
-      <c r="G18" s="70"/>
+      <c r="G18" s="83"/>
     </row>
     <row r="19" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="78"/>
+      <c r="A19" s="70"/>
       <c r="B19" s="75"/>
       <c r="C19" s="25">
         <v>52734</v>
@@ -1449,12 +1453,12 @@
         <v>52783</v>
       </c>
       <c r="F19" s="75"/>
-      <c r="G19" s="71"/>
+      <c r="G19" s="84"/>
     </row>
     <row r="20" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="79"/>
+      <c r="A20" s="71"/>
       <c r="B20" s="75"/>
-      <c r="C20" s="72"/>
+      <c r="C20" s="85"/>
       <c r="E20" s="22" t="s">
         <v>7</v>
       </c>
@@ -1462,9 +1466,9 @@
       <c r="G20" s="51"/>
     </row>
     <row r="21" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="80"/>
+      <c r="A21" s="72"/>
       <c r="B21" s="75"/>
-      <c r="C21" s="73"/>
+      <c r="C21" s="86"/>
       <c r="E21" s="22" t="s">
         <v>8</v>
       </c>
@@ -1472,7 +1476,7 @@
       <c r="G21" s="51"/>
     </row>
     <row r="22" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="81"/>
+      <c r="A22" s="73"/>
       <c r="B22" s="76"/>
       <c r="C22" s="26"/>
       <c r="E22" s="52"/>
@@ -1506,7 +1510,7 @@
   </sheetPr>
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
@@ -1515,7 +1519,7 @@
     <col min="1" max="5" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="46.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="87" t="s">
         <v>13</v>
       </c>
@@ -1524,7 +1528,7 @@
       <c r="D1" s="88"/>
       <c r="E1" s="89"/>
     </row>
-    <row r="2" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="90" t="s">
         <v>14</v>
       </c>
@@ -1533,7 +1537,7 @@
       <c r="D2" s="91"/>
       <c r="E2" s="92"/>
     </row>
-    <row r="3" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="53" t="s">
         <v>15</v>
       </c>
@@ -1638,7 +1642,7 @@
       <c r="K9" s="59"/>
       <c r="L9" s="59"/>
     </row>
-    <row r="10" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="61" t="s">
         <v>22</v>
       </c>
@@ -1686,7 +1690,7 @@
       <c r="K12" s="59"/>
       <c r="L12" s="59"/>
     </row>
-    <row r="13" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="55" t="s">
         <v>25</v>
       </c>
@@ -1702,7 +1706,7 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="55" t="s">
         <v>26</v>
       </c>
@@ -1718,7 +1722,7 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="55" t="s">
         <v>27</v>
       </c>
@@ -1734,7 +1738,7 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="62"/>
       <c r="D16" s="1"/>

</xml_diff>